<commit_message>
Added Excel Data fetching into RestAssured
</commit_message>
<xml_diff>
--- a/ExcelDemoData.xlsx
+++ b/ExcelDemoData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cdd5ec8174029c47/Desktop/ApiFramework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{7535A586-DDA0-4CBD-9531-9818CF55E7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11197012-CEB2-445D-9E61-7C274BC7DD51}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{7535A586-DDA0-4CBD-9531-9818CF55E7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68481E96-31AE-47AD-8B89-209A258A5093}"/>
   <bookViews>
-    <workbookView xWindow="-25965" yWindow="4485" windowWidth="17280" windowHeight="8880" xr2:uid="{F37DD495-51E0-4503-9F67-BCDA3F052238}"/>
+    <workbookView minimized="1" xWindow="-25965" yWindow="4485" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{F37DD495-51E0-4503-9F67-BCDA3F052238}"/>
   </bookViews>
   <sheets>
     <sheet name="testData" sheetId="1" r:id="rId1"/>
-    <sheet name="sample" sheetId="2" r:id="rId2"/>
+    <sheet name="Library" sheetId="2" r:id="rId2"/>
     <sheet name="demo" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Testcases</t>
   </si>
@@ -74,9 +74,6 @@
     <t>dcd</t>
   </si>
   <si>
-    <t>cdsc</t>
-  </si>
-  <si>
     <t>dcas</t>
   </si>
   <si>
@@ -90,13 +87,58 @@
   </si>
   <si>
     <t>Data3</t>
+  </si>
+  <si>
+    <t>31/10/2025</t>
+  </si>
+  <si>
+    <t>Keys</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>aisle</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>Appium</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Api</t>
+  </si>
+  <si>
+    <t>bcd</t>
+  </si>
+  <si>
+    <t>efg</t>
+  </si>
+  <si>
+    <t>hij</t>
+  </si>
+  <si>
+    <t>John Luther</t>
+  </si>
+  <si>
+    <t>John Zachria</t>
+  </si>
+  <si>
+    <t>John Samuel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +150,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,9 +181,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,32 +526,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E34ED06-F291-42FE-8046-321F66495F50}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -513,21 +566,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -538,10 +594,10 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -552,7 +608,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -563,12 +619,91 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FB32D1-8614-4801-B8F8-EDCA6B8D1584}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3">
+        <v>223</v>
+      </c>
+      <c r="C4" s="3">
+        <v>334</v>
+      </c>
+      <c r="D4" s="3">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>